<commit_message>
Added RESOURCELINK data source in ODBC.INI to unify naming across environments.
</commit_message>
<xml_diff>
--- a/DEV.xlsx
+++ b/DEV.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="423">
   <si>
     <t>Queue Name</t>
   </si>
@@ -1290,6 +1290,12 @@
   </si>
   <si>
     <t>Movers and transfers database (P36)</t>
+  </si>
+  <si>
+    <t>RESOURCELINK</t>
+  </si>
+  <si>
+    <t>Attempt to standardise the DSN across environments.</t>
   </si>
 </sst>
 </file>
@@ -2656,10 +2662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,402 +2716,424 @@
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>45</v>
+        <v>421</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="D3" s="22" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A3," -u ",B3," -p ",C3)</f>
-        <v>mqsisetdbparms brk0002d -n ESBCONF -u wmbadmin -p d5FZg2E9i9dGnChE4w1q</v>
+        <v>mqsisetdbparms brk0002d -n RESOURCELINK -u CMTEST -p jm08_cmt</v>
       </c>
       <c r="F3" s="22" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A3)</f>
-        <v>mqsicvp brk0002d -n ESBCONF</v>
+        <v>mqsicvp brk0002d -n RESOURCELINK</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>162</v>
+        <v>46</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>40</v>
+        <v>147</v>
       </c>
       <c r="D4" s="22" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A4," -u ",B4," -p ",C4)</f>
-        <v>mqsisetdbparms brk0002d -n BPMDB -u bpmdbusr -p b0z2kh95</v>
+        <v>mqsisetdbparms brk0002d -n ESBCONF -u wmbadmin -p d5FZg2E9i9dGnChE4w1q</v>
       </c>
       <c r="F4" s="22" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A4)</f>
+        <v>mqsicvp brk0002d -n ESBCONF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A5," -u ",B5," -p ",C5)</f>
+        <v>mqsisetdbparms brk0002d -n BPMDB -u bpmdbusr -p b0z2kh95</v>
+      </c>
+      <c r="F5" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A5)</f>
         <v>mqsicvp brk0002d -n BPMDB</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A6," -u ",B6," -p ",C6)</f>
-        <v>mqsisetdbparms brk0002d -n STATSNX_TEST -u statsnx -p statsnx</v>
-      </c>
-      <c r="F6" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A6)</f>
-        <v>mqsicvp brk0002d -n STATSNX_TEST</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>109</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="D7" s="22" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A7," -u ",B7," -p ",C7)</f>
-        <v>mqsisetdbparms brk0002d -n STATSNX_LIVE -u statsnx -p R3ms09_1</v>
+        <v>mqsisetdbparms brk0002d -n STATSNX_TEST -u statsnx -p statsnx</v>
       </c>
       <c r="F7" s="22" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A7)</f>
+        <v>mqsicvp brk0002d -n STATSNX_TEST</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A8," -u ",B8," -p ",C8)</f>
+        <v>mqsisetdbparms brk0002d -n STATSNX_LIVE -u statsnx -p R3ms09_1</v>
+      </c>
+      <c r="F8" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A8)</f>
         <v>mqsicvp brk0002d -n STATSNX_LIVE</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H8" s="22" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A8," -u ",B8," -p ",C8)</f>
-        <v>mqsisetdbparms brk0002d -n CFRS_LIVE -u cfrs_live -p cfrs_live</v>
-      </c>
-      <c r="F8" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A8)</f>
-        <v>mqsicvp brk0002d -n CFRS_LIVE</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D9" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A9," -u ",B9," -p ",C9)</f>
-        <v>mqsisetdbparms brk0002d -n RRRED -u RRRED -p rrred</v>
+        <v>mqsisetdbparms brk0002d -n CFRS_LIVE -u cfrs_live -p cfrs_live</v>
       </c>
       <c r="F9" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A9)</f>
-        <v>mqsicvp brk0002d -n RRRED</v>
+        <v>mqsicvp brk0002d -n CFRS_LIVE</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D10" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A10," -u ",B10," -p ",C10)</f>
-        <v>mqsisetdbparms brk0002d -n DM_CADM -u DM_CADM -p dm_cadm</v>
+        <v>mqsisetdbparms brk0002d -n RRRED -u RRRED -p rrred</v>
       </c>
       <c r="F10" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A10)</f>
+        <v>mqsicvp brk0002d -n RRRED</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A11," -u ",B11," -p ",C11)</f>
+        <v>mqsisetdbparms brk0002d -n DM_CADM -u DM_CADM -p dm_cadm</v>
+      </c>
+      <c r="F11" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A11)</f>
         <v>mqsicvp brk0002d -n DM_CADM</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="13" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B13" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C13" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="D12" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A12," -u ",B12," -p ",C12)</f>
+      <c r="D13" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A13," -u ",B13," -p ",C13)</f>
         <v>mqsisetdbparms brk0002d -n PERF -u ywzv -p P6HBSAP</v>
       </c>
-      <c r="F12" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A12)</f>
+      <c r="F13" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A13)</f>
         <v>mqsicvp brk0002d -n PERF</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="17" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B17" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C17" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="D16" s="25" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A16," -u ",B16," -p ",C16)</f>
+      <c r="D17" s="25" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A17," -u ",B17," -p ",C17)</f>
         <v>mqsisetdbparms brk0002d -n RECRUITMENT_DEV -u rec_userd -p Recuserd999</v>
       </c>
-      <c r="F16" s="25" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A16)</f>
+      <c r="F17" s="25" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A17)</f>
         <v>mqsicvp brk0002d -n RECRUITMENT_DEV</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+    <row r="21" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+    <row r="22" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B22" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="25" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A21," -u ",B21," -p ",C21)</f>
+      <c r="D22" s="25" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A22," -u ",B22," -p ",C22)</f>
         <v>mqsisetdbparms brk0002d -n STEP_TEST -u STEP -p h53ks!f</v>
       </c>
-      <c r="F21" s="25" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A21)</f>
+      <c r="F22" s="25" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A22)</f>
         <v>mqsicvp brk0002d -n STEP_TEST</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="23" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A23," -u ",B23," -p ",C23)</f>
-        <v>mqsisetdbparms brk0002d -n STEP -u STEP -p h53ks!f</v>
-      </c>
-      <c r="F23" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A23)</f>
-        <v>mqsicvp brk0002d -n STEP</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>165</v>
+        <v>105</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="D24" s="22" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A24," -u ",B24," -p ",C24)</f>
-        <v>mqsisetdbparms brk0002d -n STEP_SS -u step_userd -p Stepuserd999</v>
+        <v>mqsisetdbparms brk0002d -n STEP -u STEP -p h53ks!f</v>
       </c>
       <c r="F24" s="22" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A24)</f>
+        <v>mqsicvp brk0002d -n STEP</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A25," -u ",B25," -p ",C25)</f>
+        <v>mqsisetdbparms brk0002d -n STEP_SS -u step_userd -p Stepuserd999</v>
+      </c>
+      <c r="F25" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A25)</f>
         <v>mqsicvp brk0002d -n STEP_SS</v>
       </c>
-      <c r="H24" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="D26" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A26," -u ",B26," -p ",C26)</f>
-        <v>mqsisetdbparms brk0002d -n METER_READINGS -u step_userd -p Stepuserd999</v>
-      </c>
-      <c r="F26" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A26)</f>
-        <v>mqsicvp brk0002d -n METER_READINGS</v>
-      </c>
-      <c r="H26" s="22" t="s">
+      <c r="H25" s="22" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>166</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>321</v>
+        <v>167</v>
       </c>
       <c r="D27" s="22" t="str">
         <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A27," -u ",B27," -p ",C27)</f>
-        <v>mqsisetdbparms brk0002d -n TENSORNET -u step_userd -p 5t3PteamD</v>
+        <v>mqsisetdbparms brk0002d -n METER_READINGS -u step_userd -p Stepuserd999</v>
       </c>
       <c r="F27" s="22" t="str">
         <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A27)</f>
-        <v>mqsicvp brk0002d -n TENSORNET</v>
+        <v>mqsicvp brk0002d -n METER_READINGS</v>
       </c>
       <c r="H27" s="22" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+    <row r="28" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="D28" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A28," -u ",B28," -p ",C28)</f>
+        <v>mqsisetdbparms brk0002d -n TENSORNET -u step_userd -p 5t3PteamD</v>
+      </c>
+      <c r="F28" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A28)</f>
+        <v>mqsicvp brk0002d -n TENSORNET</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C30" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A29," -u ",B29," -p ",C29)</f>
+      <c r="D30" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A30," -u ",B30," -p ",C30)</f>
         <v>mqsisetdbparms brk0002d -n MBRECORD -u wmbadmin -p d5FZg2E9i9dGnChE4w1q</v>
       </c>
-      <c r="F29" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A29)</f>
+      <c r="F30" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A30)</f>
         <v>mqsicvp brk0002d -n MBRECORD</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+    <row r="32" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
         <v>373</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B32" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C32" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D31" s="34" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A31," -u ",B31," -p ",C31)</f>
+      <c r="D32" s="34" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A32," -u ",B32," -p ",C32)</f>
         <v>mqsisetdbparms brk0002d -n STEP_OCP -u step_userd -p Stepuserd999</v>
       </c>
-      <c r="F31" s="34" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A31)</f>
+      <c r="F32" s="34" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A32)</f>
         <v>mqsicvp brk0002d -n STEP_OCP</v>
       </c>
-      <c r="H31" s="34" t="s">
+      <c r="H32" s="34" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+    <row r="33" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
         <v>374</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B33" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C33" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D32" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A32," -u ",B32," -p ",C32)</f>
+      <c r="D33" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A33," -u ",B33," -p ",C33)</f>
         <v>mqsisetdbparms brk0002d -n IRSPLUS -u step_userd -p Stepuserd999</v>
       </c>
-      <c r="F32" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A32)</f>
+      <c r="F33" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A33)</f>
         <v>mqsicvp brk0002d -n IRSPLUS</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H33" s="22" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+    <row r="35" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B35" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C35" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A34," -u ",B34," -p ",C34)</f>
+      <c r="D35" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A35," -u ",B35," -p ",C35)</f>
         <v>mqsisetdbparms brk0002d -n GartanRDS -u step_userd -p Stepuserd999</v>
       </c>
-      <c r="F34" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A34)</f>
+      <c r="F35" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A35)</f>
         <v>mqsicvp brk0002d -n GartanRDS</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H35" s="22" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+    <row r="37" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B37" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C37" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D36" s="22" t="str">
-        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A36," -u ",B36," -p ",C36)</f>
+      <c r="D37" s="22" t="str">
+        <f>CONCATENATE( "mqsisetdbparms ",ConfigData!$D$4," -n ",A37," -u ",B37," -p ",C37)</f>
         <v>mqsisetdbparms brk0002d -n TRANSFERS -u step_userd -p Stepuserd999</v>
       </c>
-      <c r="F36" s="22" t="str">
-        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A36)</f>
+      <c r="F37" s="22" t="str">
+        <f>CONCATENATE( "mqsicvp ",ConfigData!$D$4," -n ",A37)</f>
         <v>mqsicvp brk0002d -n TRANSFERS</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H37" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I37" s="22" t="s">
         <v>420</v>
       </c>
     </row>

</xml_diff>